<commit_message>
updated font size of created .ass files
</commit_message>
<xml_diff>
--- a/data/translation_times.xlsx
+++ b/data/translation_times.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HexMa\Desktop\repos\translator-helper\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8340A24-81AB-438D-881E-C2BF7F98FD32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED0DB4E7-560C-47B0-AFE6-91C0D7758BE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{50C1EBFE-BD10-47AD-808E-F15717A1EC41}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{50C1EBFE-BD10-47AD-808E-F15717A1EC41}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>video</t>
   </si>
@@ -72,6 +72,9 @@
   </si>
   <si>
     <t>gakumas lilja bond step 2</t>
+  </si>
+  <si>
+    <t>makeine vol2.1</t>
   </si>
 </sst>
 </file>
@@ -79,7 +82,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.000000"/>
+    <numFmt numFmtId="164" formatCode="0.000000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -113,7 +116,7 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -449,10 +452,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B2B118A-139E-42B7-BCC2-032941E226DF}">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -556,6 +559,40 @@
         <v>1.5173764072442487E-4</v>
       </c>
     </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>10</v>
+      </c>
+      <c r="D4">
+        <v>45</v>
+      </c>
+      <c r="E4">
+        <v>331</v>
+      </c>
+      <c r="F4" s="3">
+        <v>4569</v>
+      </c>
+      <c r="G4" s="1">
+        <f>F4/E4</f>
+        <v>13.803625377643504</v>
+      </c>
+      <c r="H4">
+        <v>3</v>
+      </c>
+      <c r="I4">
+        <v>0.92</v>
+      </c>
+      <c r="J4" s="2">
+        <f>I4/F4</f>
+        <v>2.0135697089078574E-4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
translating subs now uses sub length if available
</commit_message>
<xml_diff>
--- a/data/translation_times.xlsx
+++ b/data/translation_times.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HexMa\Desktop\repos\translator-helper\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB9F2F1F-F745-47B2-9519-BD944798EA80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F21F0077-6EB5-44D8-9FB1-F2D65D9A2328}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{50C1EBFE-BD10-47AD-808E-F15717A1EC41}"/>
+    <workbookView xWindow="28680" yWindow="-945" windowWidth="29040" windowHeight="15720" xr2:uid="{50C1EBFE-BD10-47AD-808E-F15717A1EC41}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,8 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="23">
   <si>
     <t>video</t>
   </si>
@@ -90,6 +88,21 @@
   </si>
   <si>
     <t>total lines:</t>
+  </si>
+  <si>
+    <t>gakumas lilja hakusen</t>
+  </si>
+  <si>
+    <t>model</t>
+  </si>
+  <si>
+    <t>gpt-4o</t>
+  </si>
+  <si>
+    <t>gakumas lilja kamurogiku</t>
+  </si>
+  <si>
+    <t>gakumas lilja sakura photograph</t>
   </si>
 </sst>
 </file>
@@ -467,250 +480,392 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B2B118A-139E-42B7-BCC2-032941E226DF}">
-  <dimension ref="A1:N6"/>
+  <dimension ref="A1:O9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="8.28515625" customWidth="1"/>
     <col min="6" max="6" width="9.140625" style="3"/>
-    <col min="7" max="7" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5703125" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
-        <v>3</v>
-      </c>
       <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
-      <c r="B2">
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2">
         <v>0</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>23</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>36</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>935</v>
       </c>
-      <c r="F2" s="3">
+      <c r="G2" s="3">
         <v>15967</v>
       </c>
-      <c r="G2" s="1">
-        <f>F2/E2</f>
+      <c r="H2" s="1">
+        <f t="shared" ref="H2:H9" si="0">G2/F2</f>
         <v>17.077005347593584</v>
       </c>
-      <c r="H2">
-        <v>3</v>
-      </c>
-      <c r="I2" s="1">
+      <c r="I2">
+        <v>3</v>
+      </c>
+      <c r="J2" s="1">
         <f>4.98-2.58</f>
         <v>2.4000000000000004</v>
       </c>
-      <c r="J2" s="2">
-        <f>I2/F2</f>
+      <c r="K2" s="2">
+        <f t="shared" ref="K2:K9" si="1">J2/G2</f>
         <v>1.5031001440470973E-4</v>
       </c>
-      <c r="K2">
-        <f>I2/E2</f>
+      <c r="L2">
+        <f>J2/F2</f>
         <v>2.5668449197860967E-3</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>16</v>
       </c>
-      <c r="N2">
-        <f>AVERAGE(K:K)</f>
-        <v>2.688348835024694E-3</v>
+      <c r="O2">
+        <f>AVERAGE(L:L)</f>
+        <v>2.6489955536699739E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
-      <c r="B3">
+      <c r="B3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3">
         <v>0</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>705</v>
       </c>
-      <c r="F3" s="3">
+      <c r="G3" s="3">
         <v>10215</v>
       </c>
-      <c r="G3" s="1">
-        <f>F3/E3</f>
+      <c r="H3" s="1">
+        <f t="shared" si="0"/>
         <v>14.48936170212766</v>
       </c>
-      <c r="H3">
-        <v>3</v>
-      </c>
-      <c r="I3" s="1">
+      <c r="I3">
+        <v>3</v>
+      </c>
+      <c r="J3" s="1">
         <v>1.55</v>
       </c>
-      <c r="J3" s="2">
-        <f>I3/F3</f>
+      <c r="K3" s="2">
+        <f t="shared" si="1"/>
         <v>1.5173764072442487E-4</v>
       </c>
-      <c r="K3">
-        <f t="shared" ref="K3:K6" si="0">I3/E3</f>
+      <c r="L3">
+        <f t="shared" ref="L3:L9" si="2">J3/F3</f>
         <v>2.1985815602836882E-3</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>17</v>
       </c>
-      <c r="N3">
-        <f>SUM(E:E)</f>
-        <v>2570</v>
+      <c r="O3">
+        <f>SUM(F:F)</f>
+        <v>3158</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>12</v>
       </c>
-      <c r="B4">
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4">
         <v>0</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>10</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>45</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>331</v>
       </c>
-      <c r="F4" s="3">
+      <c r="G4" s="3">
         <v>4569</v>
       </c>
-      <c r="G4" s="1">
-        <f>F4/E4</f>
+      <c r="H4" s="1">
+        <f t="shared" si="0"/>
         <v>13.803625377643504</v>
       </c>
-      <c r="H4">
-        <v>3</v>
-      </c>
       <c r="I4">
+        <v>3</v>
+      </c>
+      <c r="J4">
         <v>0.92</v>
       </c>
-      <c r="J4" s="2">
-        <f>I4/F4</f>
+      <c r="K4" s="2">
+        <f t="shared" si="1"/>
         <v>2.0135697089078574E-4</v>
       </c>
-      <c r="K4">
-        <f t="shared" si="0"/>
+      <c r="L4">
+        <f t="shared" si="2"/>
         <v>2.7794561933534743E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>13</v>
       </c>
-      <c r="B5">
+      <c r="B5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5">
         <v>0</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>8</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>35</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>248</v>
       </c>
-      <c r="F5" s="3">
+      <c r="G5" s="3">
         <v>3496</v>
       </c>
-      <c r="G5" s="1">
-        <f>F5/E5</f>
+      <c r="H5" s="1">
+        <f t="shared" si="0"/>
         <v>14.096774193548388</v>
       </c>
-      <c r="H5">
-        <v>3</v>
-      </c>
       <c r="I5">
+        <v>3</v>
+      </c>
+      <c r="J5">
         <v>0.77</v>
       </c>
-      <c r="J5" s="2">
-        <f>I5/F5</f>
+      <c r="K5" s="2">
+        <f t="shared" si="1"/>
         <v>2.2025171624713959E-4</v>
       </c>
-      <c r="K5">
-        <f t="shared" si="0"/>
+      <c r="L5">
+        <f t="shared" si="2"/>
         <v>3.1048387096774192E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>14</v>
       </c>
-      <c r="B6">
+      <c r="B6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6">
         <v>0</v>
       </c>
-      <c r="C6">
+      <c r="D6">
         <v>11</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>26</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>351</v>
       </c>
-      <c r="F6" s="3">
+      <c r="G6" s="3">
         <v>4351</v>
       </c>
-      <c r="G6" s="1">
-        <f>F6/E6</f>
+      <c r="H6" s="1">
+        <f t="shared" si="0"/>
         <v>12.396011396011396</v>
       </c>
-      <c r="H6">
-        <v>3</v>
-      </c>
       <c r="I6">
+        <v>3</v>
+      </c>
+      <c r="J6">
         <v>0.98</v>
       </c>
-      <c r="J6" s="2">
-        <f>I6/F6</f>
+      <c r="K6" s="2">
+        <f t="shared" si="1"/>
         <v>2.2523557802803953E-4</v>
       </c>
-      <c r="K6">
+      <c r="L6">
+        <f t="shared" si="2"/>
+        <v>2.7920227920227919E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>3</v>
+      </c>
+      <c r="E7">
+        <v>57</v>
+      </c>
+      <c r="F7">
+        <v>166</v>
+      </c>
+      <c r="G7" s="3">
+        <v>2283</v>
+      </c>
+      <c r="H7" s="1">
         <f t="shared" si="0"/>
-        <v>2.7920227920227919E-3</v>
+        <v>13.753012048192771</v>
+      </c>
+      <c r="I7">
+        <v>3</v>
+      </c>
+      <c r="J7">
+        <v>0.38</v>
+      </c>
+      <c r="K7" s="2">
+        <f t="shared" si="1"/>
+        <v>1.6644765659220326E-4</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="2"/>
+        <v>2.2891566265060242E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>4</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8" s="3">
+        <v>162</v>
+      </c>
+      <c r="G8" s="3">
+        <v>2667</v>
+      </c>
+      <c r="H8" s="1">
+        <f t="shared" si="0"/>
+        <v>16.462962962962962</v>
+      </c>
+      <c r="I8">
+        <v>3</v>
+      </c>
+      <c r="J8">
+        <v>0.38</v>
+      </c>
+      <c r="K8" s="2">
+        <f t="shared" si="1"/>
+        <v>1.4248218972628423E-4</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="2"/>
+        <v>2.345679012345679E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>9</v>
+      </c>
+      <c r="E9">
+        <v>42</v>
+      </c>
+      <c r="F9" s="3">
+        <v>260</v>
+      </c>
+      <c r="G9" s="3">
+        <v>4231</v>
+      </c>
+      <c r="H9" s="1">
+        <f t="shared" si="0"/>
+        <v>16.273076923076925</v>
+      </c>
+      <c r="I9">
+        <v>3</v>
+      </c>
+      <c r="J9">
+        <v>0.81</v>
+      </c>
+      <c r="K9" s="2">
+        <f t="shared" si="1"/>
+        <v>1.9144410304892462E-4</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="2"/>
+        <v>3.1153846153846158E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
refactor: created interfaces for both audio transcription and llm models in backend.
- abstracted llm usage to hopefully make it easier to integrate a local llm instead of relying on open ai api
- updated frontend settings page
- removed web context and tavily api since they're not as useful as I had hoped
- deleted old streamlit version files
</commit_message>
<xml_diff>
--- a/data/translation_times.xlsx
+++ b/data/translation_times.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repos\translator-helper\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B10E1DF4-BE9F-4D85-9B5D-E25D56BB1E36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F9F29EC-D8BD-42D8-B1AE-8978707B9DE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-975" windowWidth="29040" windowHeight="15720" xr2:uid="{50C1EBFE-BD10-47AD-808E-F15717A1EC41}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{50C1EBFE-BD10-47AD-808E-F15717A1EC41}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="29">
   <si>
     <t>video</t>
   </si>
@@ -112,6 +112,15 @@
   </si>
   <si>
     <t>gakumas lilja atmosphere</t>
+  </si>
+  <si>
+    <t>gakumas lilja white night white wish</t>
+  </si>
+  <si>
+    <t>gakumas</t>
+  </si>
+  <si>
+    <t>gpt-4.1-mini</t>
   </si>
 </sst>
 </file>
@@ -489,10 +498,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B2B118A-139E-42B7-BCC2-032941E226DF}">
-  <dimension ref="A1:O12"/>
+  <dimension ref="A1:O14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+      <selection activeCell="R16" sqref="R16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -563,7 +572,7 @@
         <v>15967</v>
       </c>
       <c r="H2" s="1">
-        <f t="shared" ref="H2:H12" si="0">G2/F2</f>
+        <f t="shared" ref="H2:H11" si="0">G2/F2</f>
         <v>17.077005347593584</v>
       </c>
       <c r="I2">
@@ -574,7 +583,7 @@
         <v>2.4000000000000004</v>
       </c>
       <c r="K2" s="2">
-        <f t="shared" ref="K2:K12" si="1">J2/G2</f>
+        <f t="shared" ref="K2:K13" si="1">J2/G2</f>
         <v>1.5031001440470973E-4</v>
       </c>
       <c r="L2">
@@ -586,7 +595,7 @@
       </c>
       <c r="O2">
         <f>AVERAGE(L:L)</f>
-        <v>2.691009861742576E-3</v>
+        <v>2.5487497783481801E-3</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -620,7 +629,7 @@
         <v>1.5173764072442487E-4</v>
       </c>
       <c r="L3">
-        <f t="shared" ref="L3:L12" si="2">J3/F3</f>
+        <f t="shared" ref="L3:L13" si="2">J3/F3</f>
         <v>2.1985815602836882E-3</v>
       </c>
       <c r="N3" t="s">
@@ -628,7 +637,7 @@
       </c>
       <c r="O3">
         <f>SUM(F:F)</f>
-        <v>3704</v>
+        <v>4636</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
@@ -982,7 +991,7 @@
         <v>2620</v>
       </c>
       <c r="H12" s="1">
-        <f t="shared" si="0"/>
+        <f>G12/F12</f>
         <v>16.073619631901842</v>
       </c>
       <c r="I12">
@@ -998,6 +1007,89 @@
       <c r="L12">
         <f t="shared" si="2"/>
         <v>2.7607361963190185E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>9</v>
+      </c>
+      <c r="E13">
+        <v>18</v>
+      </c>
+      <c r="F13" s="3">
+        <v>242</v>
+      </c>
+      <c r="G13" s="3">
+        <v>5706</v>
+      </c>
+      <c r="H13" s="1">
+        <f>G13/F13</f>
+        <v>23.578512396694215</v>
+      </c>
+      <c r="I13">
+        <v>3</v>
+      </c>
+      <c r="J13">
+        <v>0.42</v>
+      </c>
+      <c r="K13" s="2">
+        <f t="shared" si="1"/>
+        <v>7.3606729758149308E-5</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="2"/>
+        <v>1.7355371900826446E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>53</v>
+      </c>
+      <c r="E14">
+        <v>38</v>
+      </c>
+      <c r="F14" s="3">
+        <v>690</v>
+      </c>
+      <c r="G14" s="3">
+        <v>16039</v>
+      </c>
+      <c r="H14" s="1">
+        <f>G14/F14</f>
+        <v>23.244927536231884</v>
+      </c>
+      <c r="I14">
+        <v>3</v>
+      </c>
+      <c r="J14">
+        <f>1.49-0.25</f>
+        <v>1.24</v>
+      </c>
+      <c r="K14" s="2">
+        <f t="shared" ref="K14" si="3">J14/G14</f>
+        <v>7.7311553089344715E-5</v>
+      </c>
+      <c r="L14">
+        <f t="shared" ref="L14" si="4">J14/F14</f>
+        <v>1.7971014492753623E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>